<commit_message>
updated to allow for app url parameters which will be used as question and answers to the Survey123 form
</commit_message>
<xml_diff>
--- a/assets/APL_Ookla_Survey.xlsx
+++ b/assets/APL_Ookla_Survey.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F8A4F5C8-41EA-4A80-864B-323245AC7C28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66AF9ED7-01E8-4CE8-86C1-74843EF7D4EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="542" xr2:uid="{C50DDC91-227D-4C28-807B-6890084E472E}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="525" xr2:uid="{C50DDC91-227D-4C28-807B-6890084E472E}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="10" r:id="rId1"/>
@@ -5063,7 +5063,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{E6D8AB08-FCF5-4248-A5AD-A4193EF46E16}"/>
   </cellStyles>
-  <dxfs count="38">
+  <dxfs count="31">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -5101,76 +5101,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5618,7 +5548,7 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Table Style 1" pivot="0" count="1" xr9:uid="{1BE14770-CAC1-4133-864C-9B15C6DBF7E4}">
-      <tableStyleElement type="wholeTable" dxfId="37"/>
+      <tableStyleElement type="wholeTable" dxfId="30"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -5698,7 +5628,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{E8BCF28F-4446-420A-A249-4C129790FE67}" name="tblSurvey" displayName="tblSurvey" ref="A1:AE102" totalsRowShown="0" headerRowDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{E8BCF28F-4446-420A-A249-4C129790FE67}" name="tblSurvey" displayName="tblSurvey" ref="A1:AE102" totalsRowShown="0" headerRowDxfId="29">
   <autoFilter ref="A1:AE102" xr:uid="{04CAF01F-613A-48AF-A687-EDBD4018AB46}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -5763,14 +5693,14 @@
     <tableColumn id="28" xr3:uid="{F14FFEBF-C213-41AB-B833-A4BF25A2713D}" name="body::accuracyThreshold"/>
     <tableColumn id="29" xr3:uid="{D186257A-598B-4B13-AD72-3E3100031F84}" name="bind::esri:warning"/>
     <tableColumn id="30" xr3:uid="{D3A8FAD9-76DE-48F0-984D-1369BA71CBB1}" name="bind::esri:warning_message"/>
-    <tableColumn id="31" xr3:uid="{F4DD4A89-AD33-420B-822D-7C4247F01315}" name="bind::saveIncomplete" dataDxfId="35"/>
+    <tableColumn id="31" xr3:uid="{F4DD4A89-AD33-420B-822D-7C4247F01315}" name="bind::saveIncomplete" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EDEF4087-4080-4F8E-89ED-74C844BA4B83}" name="tblQuestionTypes" displayName="tblQuestionTypes" ref="A1:D29" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EDEF4087-4080-4F8E-89ED-74C844BA4B83}" name="tblQuestionTypes" displayName="tblQuestionTypes" ref="A1:D29" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
   <autoFilter ref="A1:D29" xr:uid="{D2BB9380-7DBC-430E-9367-0B6804959231}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -5778,23 +5708,23 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{5569A296-72EF-49F5-AAE4-3D3F6FCD8CD5}" name="Question type" dataDxfId="32"/>
-    <tableColumn id="2" xr3:uid="{446F971D-0AFF-4279-840E-A2C6A8D1B118}" name="Description" dataDxfId="31"/>
-    <tableColumn id="3" xr3:uid="{1B8C18C7-2F93-4C0A-9671-6F73913CFB2C}" name="Field app" dataDxfId="30"/>
-    <tableColumn id="4" xr3:uid="{8C8D6D5B-C5A1-4E4C-8E30-41B268807ADA}" name="Web app" dataDxfId="29"/>
+    <tableColumn id="1" xr3:uid="{5569A296-72EF-49F5-AAE4-3D3F6FCD8CD5}" name="Question type" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{446F971D-0AFF-4279-840E-A2C6A8D1B118}" name="Description" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{1B8C18C7-2F93-4C0A-9671-6F73913CFB2C}" name="Field app" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{8C8D6D5B-C5A1-4E4C-8E30-41B268807ADA}" name="Web app" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8FDC4328-13F6-48E0-972A-CDE030F598AD}" name="tblAppearances" displayName="tblAppearances" ref="A1:E30" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8FDC4328-13F6-48E0-972A-CDE030F598AD}" name="tblAppearances" displayName="tblAppearances" ref="A1:E30" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{065F66EE-AE5F-45CF-9A25-CF742F1AFBFB}" name="Appearance" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{CCB7347D-C6A5-4B25-B167-8E454B33D2A2}" name="Applies to" dataDxfId="25"/>
-    <tableColumn id="3" xr3:uid="{7E6DAC85-EAD8-43B4-9CD9-1D4600B87CC4}" name="Description" dataDxfId="24"/>
-    <tableColumn id="4" xr3:uid="{326BB996-88BE-426A-B473-DD340AB2689A}" name="Field app" dataDxfId="23"/>
-    <tableColumn id="5" xr3:uid="{DDA014E9-7F86-48E1-9CC8-9D66D7009E2F}" name="Web app" dataDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{065F66EE-AE5F-45CF-9A25-CF742F1AFBFB}" name="Appearance" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{CCB7347D-C6A5-4B25-B167-8E454B33D2A2}" name="Applies to" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{7E6DAC85-EAD8-43B4-9CD9-1D4600B87CC4}" name="Description" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{326BB996-88BE-426A-B473-DD340AB2689A}" name="Field app" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{DDA014E9-7F86-48E1-9CC8-9D66D7009E2F}" name="Web app" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -5808,8 +5738,8 @@
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{3F05F349-1A9F-403B-A3B4-24E1E9732F01}" name="Esri field types" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{E21F91EE-DEEC-4C26-8B49-009A0DA88A78}" name="Control the field type for a question in the bind::esri:fieldType column." dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{3F05F349-1A9F-403B-A3B4-24E1E9732F01}" name="Esri field types" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{E21F91EE-DEEC-4C26-8B49-009A0DA88A78}" name="Control the field type for a question in the bind::esri:fieldType column." dataDxfId="13"/>
     <tableColumn id="3" xr3:uid="{474B3189-9717-47F1-85D2-1115BEA7D318}" name="Learn more"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -5824,8 +5754,8 @@
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{8ABABCDA-565D-4DA1-AF46-EA67EE5579DE}" name="Bind types" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{DD933ECF-7EB5-4195-AA7A-8DF55FDF81CA}" name="Use in the bind::type column to overwrite default field type during a survey." dataDxfId="18"/>
+    <tableColumn id="1" xr3:uid="{8ABABCDA-565D-4DA1-AF46-EA67EE5579DE}" name="Bind types" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{DD933ECF-7EB5-4195-AA7A-8DF55FDF81CA}" name="Use in the bind::type column to overwrite default field type during a survey." dataDxfId="11"/>
     <tableColumn id="3" xr3:uid="{9672D06C-FA8E-4A81-8985-F209E2F23F4E}" name="Learn more"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -5833,12 +5763,12 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{EFADEFCE-A6FA-4E9A-9F3E-21F68ACF1AF3}" name="tblReserved" displayName="tblReserved" ref="A1:A1024" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{EFADEFCE-A6FA-4E9A-9F3E-21F68ACF1AF3}" name="tblReserved" displayName="tblReserved" ref="A1:A1024" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
   <autoFilter ref="A1:A1024" xr:uid="{35D3327E-F638-495F-922F-85E720598A97}">
     <filterColumn colId="0" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{4724A0EE-AB51-48A2-8A08-2E650EEB5F07}" name="Reserved keywords" dataDxfId="15"/>
+    <tableColumn id="1" xr3:uid="{4724A0EE-AB51-48A2-8A08-2E650EEB5F07}" name="Reserved keywords" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6146,9 +6076,9 @@
   </sheetPr>
   <dimension ref="A1:AE102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
       <pane xSplit="4" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D12" sqref="D12"/>
+      <selection pane="topRight" activeCell="A4" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6924,7 +6854,7 @@
   </sheetData>
   <dataConsolidate/>
   <conditionalFormatting sqref="B39:B102">
-    <cfRule type="duplicateValues" dxfId="14" priority="27" stopIfTrue="1"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="27" stopIfTrue="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6 B13:B38">
     <cfRule type="duplicateValues" dxfId="6" priority="3" stopIfTrue="1"/>
@@ -15852,12 +15782,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E8998AE3FF28B64CB6D4F669AA9D51A0" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="422df0d4c160c195778ac749863bddb7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="103c592b-7f21-4a3d-a5ad-3d19f0594a05" xmlns:ns4="59256956-c806-4785-8e70-c8eaf9cc67fa" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3bf9dcec39555256a866961cf4d27bdc" ns3:_="" ns4:_="">
     <xsd:import namespace="103c592b-7f21-4a3d-a5ad-3d19f0594a05"/>
@@ -16080,6 +16004,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{999E33D6-9489-4EF7-8D0C-0F39EFAB9B3C}">
   <ds:schemaRefs>
@@ -16089,15 +16019,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9DAA5817-170F-452A-A1D4-54BA992F7F2E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D5279D93-3CFA-448A-B000-65AF2AB1A330}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -16114,4 +16035,13 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9DAA5817-170F-452A-A1D4-54BA992F7F2E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>